<commit_message>
adjusted lung function timing
Next, insert vlines on categorical x-axis
</commit_message>
<xml_diff>
--- a/data-raw/lung_function.xlsx
+++ b/data-raw/lung_function.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="76">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -39,6 +39,30 @@
   </si>
   <si>
     <t xml:space="preserve">fev_pre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40_mg_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40_mg_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40_mg_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80_mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">160_mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">320_mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">480_mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">640_mg</t>
   </si>
   <si>
     <t xml:space="preserve">sal_1</t>
@@ -450,11 +474,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -534,11 +558,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -649,8 +673,8 @@
   </sheetPr>
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T17" activeCellId="0" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -697,82 +721,82 @@
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H1" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="I1" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="J1" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="K1" s="7" t="n">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="7" t="n">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="7" t="n">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="7" t="n">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="O1" s="8" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="U1" s="12" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="V1" s="12" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="W1" s="13" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="X1" s="14" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="Y1" s="15" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="Z1" s="16" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="AA1" s="16" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="AB1" s="17" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D2" s="20" t="n">
         <v>4</v>
@@ -852,13 +876,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D3" s="23" t="n">
         <v>5</v>
@@ -929,13 +953,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D4" s="20" t="n">
         <v>1</v>
@@ -1015,13 +1039,13 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D5" s="20" t="n">
         <v>3</v>
@@ -1101,13 +1125,13 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D6" s="20" t="n">
         <v>5</v>
@@ -1187,13 +1211,13 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D7" s="20" t="n">
         <v>5</v>
@@ -1273,13 +1297,13 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D8" s="20" t="n">
         <v>1</v>
@@ -1359,13 +1383,13 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>22</v>
       </c>
       <c r="D9" s="20" t="n">
         <v>3</v>
@@ -1445,13 +1469,13 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D10" s="20" t="n">
         <v>5</v>
@@ -1531,13 +1555,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D11" s="20" t="n">
         <v>4</v>
@@ -1617,13 +1641,13 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D12" s="20" t="n">
         <v>4</v>
@@ -1703,13 +1727,13 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D13" s="20" t="n">
         <v>4</v>
@@ -1789,13 +1813,13 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D14" s="20" t="n">
         <v>4</v>
@@ -1875,13 +1899,13 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D15" s="20" t="n">
         <v>5</v>
@@ -1961,13 +1985,13 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D16" s="20" t="n">
         <v>1</v>
@@ -2047,13 +2071,13 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D17" s="20" t="n">
         <v>3</v>
@@ -2133,13 +2157,13 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D18" s="20" t="n">
         <v>5</v>
@@ -2219,13 +2243,13 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D19" s="20" t="n">
         <v>3</v>
@@ -2305,13 +2329,13 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D20" s="20" t="n">
         <v>5</v>
@@ -2391,87 +2415,87 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="25" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="27" t="n">
+        <v>29</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="28" t="n">
         <v>4</v>
       </c>
       <c r="E21" s="25" t="n">
         <v>4.83</v>
       </c>
-      <c r="F21" s="27" t="n">
+      <c r="F21" s="28" t="n">
         <v>3.94</v>
       </c>
       <c r="G21" s="25" t="n">
         <v>4.01</v>
       </c>
-      <c r="H21" s="28" t="n">
+      <c r="H21" s="27" t="n">
         <v>4</v>
       </c>
-      <c r="I21" s="28" t="n">
+      <c r="I21" s="27" t="n">
         <v>3.83</v>
       </c>
-      <c r="J21" s="28" t="n">
+      <c r="J21" s="27" t="n">
         <v>3.62</v>
       </c>
-      <c r="K21" s="28" t="n">
+      <c r="K21" s="27" t="n">
         <v>4.11</v>
       </c>
-      <c r="L21" s="0" t="n">
+      <c r="L21" s="27" t="n">
         <v>3.75</v>
       </c>
-      <c r="M21" s="0" t="n">
+      <c r="M21" s="27" t="n">
         <v>3.655</v>
       </c>
-      <c r="N21" s="0" t="n">
+      <c r="N21" s="27" t="n">
         <v>3.65</v>
       </c>
       <c r="O21" s="25" t="n">
         <v>3.84</v>
       </c>
-      <c r="P21" s="28" t="n">
+      <c r="P21" s="27" t="n">
         <v>3.8</v>
       </c>
-      <c r="Q21" s="28" t="n">
+      <c r="Q21" s="27" t="n">
         <v>3.77</v>
       </c>
-      <c r="R21" s="27" t="n">
+      <c r="R21" s="28" t="n">
         <v>3.94</v>
       </c>
       <c r="S21" s="25" t="n">
         <v>4.9</v>
       </c>
-      <c r="T21" s="28" t="n">
+      <c r="T21" s="27" t="n">
         <v>118</v>
       </c>
-      <c r="U21" s="28" t="n">
+      <c r="U21" s="27" t="n">
         <v>4.06</v>
       </c>
-      <c r="V21" s="28" t="n">
+      <c r="V21" s="27" t="n">
         <v>117</v>
       </c>
-      <c r="W21" s="28" t="n">
+      <c r="W21" s="27" t="n">
         <v>84</v>
       </c>
-      <c r="X21" s="27" t="n">
+      <c r="X21" s="28" t="n">
         <v>69</v>
       </c>
       <c r="Y21" s="25" t="n">
         <v>4</v>
       </c>
-      <c r="Z21" s="28" t="n">
+      <c r="Z21" s="27" t="n">
         <v>4.38</v>
       </c>
-      <c r="AA21" s="28" t="n">
+      <c r="AA21" s="27" t="n">
         <v>3.82</v>
       </c>
-      <c r="AB21" s="27" t="n">
+      <c r="AB21" s="28" t="n">
         <v>4.11</v>
       </c>
     </row>
@@ -2522,75 +2546,75 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G1" s="31" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="I1" s="32" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J1" s="33" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="P1" s="14" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="Q1" s="15" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="R1" s="16" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="S1" s="16" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="T1" s="17" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>5</v>
@@ -2646,13 +2670,13 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="24" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D3" s="24" t="n">
         <v>4</v>
@@ -2708,13 +2732,13 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>5</v>
@@ -2770,13 +2794,13 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -2832,13 +2856,13 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D6" s="34" t="n">
         <v>2</v>
@@ -2894,13 +2918,13 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D7" s="34" t="n">
         <v>4</v>
@@ -2956,13 +2980,13 @@
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D8" s="34" t="n">
         <v>5</v>
@@ -3018,13 +3042,13 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D9" s="34" t="n">
         <v>1</v>
@@ -3080,13 +3104,13 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D10" s="34" t="n">
         <v>2</v>
@@ -3142,13 +3166,13 @@
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D11" s="34" t="n">
         <v>3</v>
@@ -3204,13 +3228,13 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D12" s="34" t="n">
         <v>5</v>
@@ -3266,13 +3290,13 @@
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D13" s="34" t="n">
         <v>3</v>
@@ -3328,13 +3352,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D14" s="34" t="n">
         <v>5</v>
@@ -3390,13 +3414,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D15" s="34" t="n">
         <v>4</v>
@@ -3452,13 +3476,13 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D16" s="34" t="n">
         <v>5</v>
@@ -3514,13 +3538,13 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D17" s="34" t="n">
         <v>1</v>
@@ -3576,13 +3600,13 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D18" s="34" t="n">
         <v>2</v>
@@ -3638,13 +3662,13 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D19" s="34" t="n">
         <v>1</v>
@@ -3700,13 +3724,13 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D20" s="34" t="n">
         <v>2</v>
@@ -3761,14 +3785,14 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="28" t="s">
-        <v>42</v>
+      <c r="A21" s="27" t="s">
+        <v>50</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>63</v>
+        <v>29</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>71</v>
       </c>
       <c r="D21" s="35" t="n">
         <v>3</v>
@@ -3776,61 +3800,61 @@
       <c r="E21" s="25" t="n">
         <v>4.85</v>
       </c>
-      <c r="F21" s="28" t="n">
+      <c r="F21" s="27" t="n">
         <v>117</v>
       </c>
-      <c r="G21" s="28" t="n">
+      <c r="G21" s="27" t="n">
         <v>3.9</v>
       </c>
-      <c r="H21" s="28" t="n">
+      <c r="H21" s="27" t="n">
         <v>113</v>
       </c>
-      <c r="I21" s="28" t="n">
+      <c r="I21" s="27" t="n">
         <v>110</v>
       </c>
-      <c r="J21" s="27" t="n">
+      <c r="J21" s="28" t="n">
         <v>76</v>
       </c>
       <c r="K21" s="25" t="n">
         <v>4.88</v>
       </c>
-      <c r="L21" s="28" t="n">
+      <c r="L21" s="27" t="n">
         <v>118</v>
       </c>
-      <c r="M21" s="28" t="n">
+      <c r="M21" s="27" t="n">
         <v>4.14</v>
       </c>
-      <c r="N21" s="28" t="n">
+      <c r="N21" s="27" t="n">
         <v>120</v>
       </c>
-      <c r="O21" s="28" t="n">
+      <c r="O21" s="27" t="n">
         <v>96</v>
       </c>
-      <c r="P21" s="27" t="n">
+      <c r="P21" s="28" t="n">
         <v>73</v>
       </c>
       <c r="Q21" s="25" t="n">
         <v>4.08</v>
       </c>
-      <c r="R21" s="28" t="n">
+      <c r="R21" s="27" t="n">
         <v>3.81</v>
       </c>
-      <c r="S21" s="28" t="n">
+      <c r="S21" s="27" t="n">
         <v>4.07</v>
       </c>
-      <c r="T21" s="27" t="n">
+      <c r="T21" s="28" t="n">
         <v>4.14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D22" s="34" t="n">
         <v>1</v>
@@ -3886,13 +3910,13 @@
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D23" s="24" t="n">
         <v>3</v>
@@ -3948,13 +3972,13 @@
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D24" s="34" t="n">
         <v>2</v>
@@ -4010,13 +4034,13 @@
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D25" s="34" t="n">
         <v>4</v>
@@ -4072,13 +4096,13 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D26" s="34" t="n">
         <v>3</v>
@@ -4134,13 +4158,13 @@
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D27" s="34" t="n">
         <v>3</v>
@@ -4196,13 +4220,13 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="19" t="s">
-        <v>21</v>
-      </c>
       <c r="C28" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D28" s="34" t="n">
         <v>2</v>
@@ -4258,13 +4282,13 @@
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D29" s="34" t="n">
         <v>4</v>
@@ -4320,13 +4344,13 @@
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D30" s="34" t="n">
         <v>3</v>
@@ -4382,13 +4406,13 @@
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D31" s="34" t="n">
         <v>1</v>
@@ -4444,13 +4468,13 @@
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D32" s="34" t="n">
         <v>1</v>
@@ -4506,13 +4530,13 @@
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D33" s="34" t="n">
         <v>1</v>
@@ -4568,13 +4592,13 @@
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D34" s="34" t="n">
         <v>1</v>
@@ -4630,13 +4654,13 @@
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D35" s="34" t="n">
         <v>3</v>
@@ -4692,13 +4716,13 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D36" s="34" t="n">
         <v>2</v>
@@ -4754,13 +4778,13 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D37" s="34" t="n">
         <v>4</v>
@@ -4816,13 +4840,13 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D38" s="34" t="n">
         <v>3</v>
@@ -4878,13 +4902,13 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D39" s="34" t="n">
         <v>4</v>
@@ -4940,13 +4964,13 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D40" s="34" t="n">
         <v>3</v>
@@ -5001,14 +5025,14 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="28" t="s">
-        <v>42</v>
+      <c r="A41" s="27" t="s">
+        <v>50</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C41" s="28" t="s">
-        <v>64</v>
+        <v>29</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>72</v>
       </c>
       <c r="D41" s="35" t="n">
         <v>1</v>
@@ -5016,61 +5040,61 @@
       <c r="E41" s="25" t="n">
         <v>4.77</v>
       </c>
-      <c r="F41" s="28" t="n">
+      <c r="F41" s="27" t="n">
         <v>115</v>
       </c>
-      <c r="G41" s="28" t="n">
+      <c r="G41" s="27" t="n">
         <v>3.92</v>
       </c>
-      <c r="H41" s="28" t="n">
+      <c r="H41" s="27" t="n">
         <v>113</v>
       </c>
-      <c r="I41" s="28" t="n">
+      <c r="I41" s="27" t="n">
         <v>99</v>
       </c>
-      <c r="J41" s="27" t="n">
+      <c r="J41" s="28" t="n">
         <v>73</v>
       </c>
       <c r="K41" s="25" t="n">
         <v>4.88</v>
       </c>
-      <c r="L41" s="28" t="n">
+      <c r="L41" s="27" t="n">
         <v>118</v>
       </c>
-      <c r="M41" s="28" t="n">
+      <c r="M41" s="27" t="n">
         <v>4.16</v>
       </c>
-      <c r="N41" s="28" t="n">
+      <c r="N41" s="27" t="n">
         <v>121</v>
       </c>
-      <c r="O41" s="28" t="n">
+      <c r="O41" s="27" t="n">
         <v>104</v>
       </c>
-      <c r="P41" s="27" t="n">
+      <c r="P41" s="28" t="n">
         <v>84</v>
       </c>
       <c r="Q41" s="25" t="n">
         <v>3.97</v>
       </c>
-      <c r="R41" s="28" t="n">
+      <c r="R41" s="27" t="n">
         <v>4.07</v>
       </c>
-      <c r="S41" s="28" t="n">
+      <c r="S41" s="27" t="n">
         <v>4.02</v>
       </c>
-      <c r="T41" s="27" t="n">
+      <c r="T41" s="28" t="n">
         <v>4.06</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D42" s="34" t="n">
         <v>2</v>
@@ -5126,13 +5150,13 @@
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="24" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D43" s="24" t="n">
         <v>1</v>
@@ -5188,13 +5212,13 @@
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D44" s="34" t="n">
         <v>4</v>
@@ -5250,13 +5274,13 @@
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D45" s="34" t="n">
         <v>2</v>
@@ -5312,13 +5336,13 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D46" s="34" t="n">
         <v>4</v>
@@ -5374,13 +5398,13 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D47" s="34" t="n">
         <v>1</v>
@@ -5436,13 +5460,13 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B48" s="19" t="s">
-        <v>21</v>
-      </c>
       <c r="C48" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D48" s="34" t="n">
         <v>4</v>
@@ -5498,13 +5522,13 @@
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D49" s="34" t="n">
         <v>2</v>
@@ -5560,13 +5584,13 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D50" s="34" t="n">
         <v>4</v>
@@ -5622,13 +5646,13 @@
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D51" s="34" t="n">
         <v>5</v>
@@ -5684,13 +5708,13 @@
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D52" s="34" t="n">
         <v>2</v>
@@ -5746,13 +5770,13 @@
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D53" s="34" t="n">
         <v>5</v>
@@ -5808,13 +5832,13 @@
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D54" s="34" t="n">
         <v>2</v>
@@ -5870,13 +5894,13 @@
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D55" s="34" t="n">
         <v>1</v>
@@ -5932,13 +5956,13 @@
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D56" s="34" t="n">
         <v>4</v>
@@ -5994,13 +6018,13 @@
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D57" s="34" t="n">
         <v>2</v>
@@ -6056,13 +6080,13 @@
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D58" s="34" t="n">
         <v>4</v>
@@ -6118,13 +6142,13 @@
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D59" s="34" t="n">
         <v>2</v>
@@ -6180,13 +6204,13 @@
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D60" s="34" t="n">
         <v>4</v>
@@ -6241,14 +6265,14 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="28" t="s">
-        <v>42</v>
+      <c r="A61" s="27" t="s">
+        <v>50</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C61" s="28" t="s">
-        <v>65</v>
+        <v>29</v>
+      </c>
+      <c r="C61" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="D61" s="35" t="n">
         <v>5</v>
@@ -6256,61 +6280,61 @@
       <c r="E61" s="25" t="n">
         <v>4.77</v>
       </c>
-      <c r="F61" s="28" t="n">
+      <c r="F61" s="27" t="n">
         <v>115</v>
       </c>
-      <c r="G61" s="28" t="n">
+      <c r="G61" s="27" t="n">
         <v>3.85</v>
       </c>
-      <c r="H61" s="28" t="n">
+      <c r="H61" s="27" t="n">
         <v>111</v>
       </c>
-      <c r="I61" s="28" t="n">
+      <c r="I61" s="27" t="n">
         <v>120</v>
       </c>
-      <c r="J61" s="27" t="n">
+      <c r="J61" s="28" t="n">
         <v>76</v>
       </c>
       <c r="K61" s="25" t="n">
         <v>4.84</v>
       </c>
-      <c r="L61" s="28" t="n">
+      <c r="L61" s="27" t="n">
         <v>117</v>
       </c>
-      <c r="M61" s="28" t="n">
+      <c r="M61" s="27" t="n">
         <v>4.14</v>
       </c>
-      <c r="N61" s="28" t="n">
+      <c r="N61" s="27" t="n">
         <v>120</v>
       </c>
-      <c r="O61" s="28" t="n">
+      <c r="O61" s="27" t="n">
         <v>117</v>
       </c>
-      <c r="P61" s="27" t="n">
+      <c r="P61" s="28" t="n">
         <v>83</v>
       </c>
       <c r="Q61" s="25" t="n">
         <v>4.03</v>
       </c>
-      <c r="R61" s="28" t="n">
+      <c r="R61" s="27" t="n">
         <v>4.09</v>
       </c>
-      <c r="S61" s="28" t="n">
+      <c r="S61" s="27" t="n">
         <v>4.26</v>
       </c>
-      <c r="T61" s="27" t="n">
+      <c r="T61" s="28" t="n">
         <v>4.07</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D62" s="34" t="n">
         <v>3</v>
@@ -6366,13 +6390,13 @@
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="24" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D63" s="24" t="n">
         <v>2</v>
@@ -6428,13 +6452,13 @@
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D64" s="34" t="n">
         <v>3</v>
@@ -6490,13 +6514,13 @@
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D65" s="34" t="n">
         <v>5</v>
@@ -6552,13 +6576,13 @@
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D66" s="34" t="n">
         <v>1</v>
@@ -6614,13 +6638,13 @@
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D67" s="34" t="n">
         <v>2</v>
@@ -6676,13 +6700,13 @@
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B68" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B68" s="19" t="s">
-        <v>21</v>
-      </c>
       <c r="C68" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D68" s="34" t="n">
         <v>3</v>
@@ -6738,13 +6762,13 @@
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D69" s="34" t="n">
         <v>5</v>
@@ -6800,13 +6824,13 @@
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D70" s="34" t="n">
         <v>1</v>
@@ -6862,13 +6886,13 @@
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D71" s="34" t="n">
         <v>2</v>
@@ -6924,13 +6948,13 @@
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D72" s="34" t="n">
         <v>3</v>
@@ -6986,13 +7010,13 @@
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D73" s="34" t="n">
         <v>2</v>
@@ -7048,13 +7072,13 @@
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D74" s="34" t="n">
         <v>3</v>
@@ -7110,13 +7134,13 @@
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D75" s="34" t="n">
         <v>2</v>
@@ -7172,13 +7196,13 @@
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D76" s="34" t="n">
         <v>3</v>
@@ -7234,13 +7258,13 @@
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D77" s="34" t="n">
         <v>5</v>
@@ -7296,13 +7320,13 @@
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D78" s="34" t="n">
         <v>1</v>
@@ -7358,13 +7382,13 @@
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D79" s="34" t="n">
         <v>5</v>
@@ -7420,13 +7444,13 @@
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D80" s="34" t="n">
         <v>1</v>
@@ -7481,14 +7505,14 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="28" t="s">
-        <v>42</v>
+      <c r="A81" s="27" t="s">
+        <v>50</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C81" s="28" t="s">
-        <v>66</v>
+        <v>29</v>
+      </c>
+      <c r="C81" s="27" t="s">
+        <v>74</v>
       </c>
       <c r="D81" s="35" t="n">
         <v>2</v>
@@ -7496,61 +7520,61 @@
       <c r="E81" s="25" t="n">
         <v>4.93</v>
       </c>
-      <c r="F81" s="28" t="n">
+      <c r="F81" s="27" t="n">
         <v>119</v>
       </c>
-      <c r="G81" s="28" t="n">
+      <c r="G81" s="27" t="n">
         <v>4.04</v>
       </c>
-      <c r="H81" s="28" t="n">
+      <c r="H81" s="27" t="n">
         <v>117</v>
       </c>
-      <c r="I81" s="28" t="n">
+      <c r="I81" s="27" t="n">
         <v>127</v>
       </c>
-      <c r="J81" s="27" t="n">
+      <c r="J81" s="28" t="n">
         <v>79</v>
       </c>
       <c r="K81" s="25" t="n">
         <v>4.8</v>
       </c>
-      <c r="L81" s="28" t="n">
+      <c r="L81" s="27" t="n">
         <v>116</v>
       </c>
-      <c r="M81" s="28" t="n">
+      <c r="M81" s="27" t="n">
         <v>3.92</v>
       </c>
-      <c r="N81" s="28" t="n">
+      <c r="N81" s="27" t="n">
         <v>113</v>
       </c>
-      <c r="O81" s="28" t="n">
+      <c r="O81" s="27" t="n">
         <v>104</v>
       </c>
-      <c r="P81" s="27" t="n">
+      <c r="P81" s="28" t="n">
         <v>79</v>
       </c>
       <c r="Q81" s="25" t="n">
         <v>3.98</v>
       </c>
-      <c r="R81" s="28" t="n">
+      <c r="R81" s="27" t="n">
         <v>4.04</v>
       </c>
-      <c r="S81" s="28" t="n">
+      <c r="S81" s="27" t="n">
         <v>4.02</v>
       </c>
-      <c r="T81" s="27" t="n">
+      <c r="T81" s="28" t="n">
         <v>3.93</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="18" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B82" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D82" s="20" t="n">
         <v>4</v>
@@ -7594,13 +7618,13 @@
     </row>
     <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="21" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B83" s="22" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C83" s="24" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D83" s="23" t="n">
         <v>5</v>
@@ -7644,13 +7668,13 @@
     </row>
     <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="18" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B84" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D84" s="20" t="n">
         <v>1</v>
@@ -7694,13 +7718,13 @@
     </row>
     <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="18" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B85" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D85" s="20" t="n">
         <v>3</v>
@@ -7744,13 +7768,13 @@
     </row>
     <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="18" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B86" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D86" s="20" t="n">
         <v>5</v>
@@ -7794,13 +7818,13 @@
     </row>
     <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="18" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B87" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D87" s="20" t="n">
         <v>5</v>
@@ -7844,13 +7868,13 @@
     </row>
     <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B88" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B88" s="19" t="s">
-        <v>21</v>
-      </c>
       <c r="C88" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D88" s="20" t="n">
         <v>1</v>
@@ -7894,13 +7918,13 @@
     </row>
     <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="18" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B89" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D89" s="20" t="n">
         <v>3</v>
@@ -7944,13 +7968,13 @@
     </row>
     <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="18" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B90" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D90" s="20" t="n">
         <v>5</v>
@@ -7994,13 +8018,13 @@
     </row>
     <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="18" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B91" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D91" s="20" t="n">
         <v>4</v>
@@ -8044,13 +8068,13 @@
     </row>
     <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="18" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B92" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D92" s="20" t="n">
         <v>4</v>
@@ -8094,13 +8118,13 @@
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="18" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B93" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D93" s="20" t="n">
         <v>4</v>
@@ -8144,13 +8168,13 @@
     </row>
     <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="18" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B94" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D94" s="20" t="n">
         <v>4</v>
@@ -8194,13 +8218,13 @@
     </row>
     <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="18" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B95" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D95" s="20" t="n">
         <v>5</v>
@@ -8244,13 +8268,13 @@
     </row>
     <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="18" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B96" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D96" s="20" t="n">
         <v>1</v>
@@ -8294,13 +8318,13 @@
     </row>
     <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="18" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D97" s="20" t="n">
         <v>3</v>
@@ -8344,13 +8368,13 @@
     </row>
     <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="18" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D98" s="20" t="n">
         <v>5</v>
@@ -8394,13 +8418,13 @@
     </row>
     <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="18" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D99" s="20" t="n">
         <v>3</v>
@@ -8444,13 +8468,13 @@
     </row>
     <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="18" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D100" s="20" t="n">
         <v>5</v>
@@ -8494,51 +8518,51 @@
     </row>
     <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="25" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B101" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C101" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="D101" s="27" t="n">
+        <v>29</v>
+      </c>
+      <c r="C101" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D101" s="28" t="n">
         <v>4</v>
       </c>
       <c r="E101" s="25" t="n">
         <v>4.83</v>
       </c>
-      <c r="G101" s="27" t="n">
+      <c r="G101" s="28" t="n">
         <v>3.94</v>
       </c>
       <c r="K101" s="25" t="n">
         <v>4.9</v>
       </c>
-      <c r="L101" s="28" t="n">
+      <c r="L101" s="27" t="n">
         <v>118</v>
       </c>
-      <c r="M101" s="28" t="n">
+      <c r="M101" s="27" t="n">
         <v>4.06</v>
       </c>
-      <c r="N101" s="28" t="n">
+      <c r="N101" s="27" t="n">
         <v>117</v>
       </c>
-      <c r="O101" s="28" t="n">
+      <c r="O101" s="27" t="n">
         <v>84</v>
       </c>
-      <c r="P101" s="27" t="n">
+      <c r="P101" s="28" t="n">
         <v>69</v>
       </c>
       <c r="Q101" s="25" t="n">
         <v>4</v>
       </c>
-      <c r="R101" s="28" t="n">
+      <c r="R101" s="27" t="n">
         <v>4.38</v>
       </c>
-      <c r="S101" s="28" t="n">
+      <c r="S101" s="27" t="n">
         <v>3.82</v>
       </c>
-      <c r="T101" s="27" t="n">
+      <c r="T101" s="28" t="n">
         <v>4.11</v>
       </c>
     </row>

</xml_diff>